<commit_message>
Added fromString class method
</commit_message>
<xml_diff>
--- a/Recipe volume to weight/conversions.xlsx
+++ b/Recipe volume to weight/conversions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bilal\source\repos\Recipe volume to weight\Recipe volume to weight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4ADCB5-BFAA-4788-9402-99B24768FB93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8FE5DD-5E17-48C9-BA14-B39ED342BED7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="-90" windowWidth="18430" windowHeight="10980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="352">
   <si>
     <t>almonds, ground</t>
   </si>
@@ -1016,9 +1016,6 @@
     <t>For eggs, egg whites, egg yolks and stick of butter unit field is left blank</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
     <t>tablespoon</t>
   </si>
   <si>
@@ -1046,9 +1043,6 @@
     <t>cup</t>
   </si>
   <si>
-    <t>Equivalent</t>
-  </si>
-  <si>
     <t>ounces</t>
   </si>
   <si>
@@ -1086,6 +1080,15 @@
   </si>
   <si>
     <t>powdered sugar</t>
+  </si>
+  <si>
+    <t>confectioner sugar</t>
+  </si>
+  <si>
+    <t>Normal ingredient name</t>
+  </si>
+  <si>
+    <t>Equivalent ingredient names</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1102,7 @@
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.0\ %"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1140,13 +1143,6 @@
     <font>
       <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1232,7 +1228,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1268,7 +1264,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1290,11 +1287,11 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1378,9 +1375,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>241300</xdr:colOff>
+          <xdr:colOff>596900</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>60325</xdr:rowOff>
+          <xdr:rowOff>101600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1826,9 +1823,9 @@
   <dimension ref="A1:AD304"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="AA234" sqref="AA234"/>
+      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -18688,8 +18685,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId6" name="TempCombo">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="1046" r:id="rId6" name="CommandButton">
+          <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>3175</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>44450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1046" r:id="rId6" name="CommandButton"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1032" r:id="rId8" name="TempCombo">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -18708,32 +18730,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1032" r:id="rId6" name="TempCombo"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1046" r:id="rId8" name="CommandButton">
-          <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>3175</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>44450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1046" r:id="rId8" name="CommandButton"/>
+        <control shapeId="1032" r:id="rId8" name="TempCombo"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18742,127 +18739,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C456A2-2442-4B14-A5A2-002CEFEDB788}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="16384" width="8.7265625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="30" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A2" s="29" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A2" s="29" t="s">
+      <c r="E2" s="29" t="s">
         <v>329</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>328</v>
-      </c>
-      <c r="C2" s="29" t="s">
+      <c r="F2" s="29" t="s">
         <v>330</v>
       </c>
-      <c r="D2" s="29" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A3" s="29" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A3" s="29" t="s">
+      <c r="D3" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="E3" s="29" t="s">
         <v>333</v>
       </c>
-      <c r="C3" s="29" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A4" s="29" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A4" s="29" t="s">
+      <c r="D4" s="29" t="s">
         <v>335</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="E4" s="29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A5" s="29" t="s">
         <v>336</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A5" s="29" t="s">
+      <c r="D5" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.6">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A6" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="D6" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="H6" s="29" t="s">
         <v>339</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="I6" s="29" t="s">
         <v>340</v>
       </c>
-      <c r="D6" s="29" t="s">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A7" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>341</v>
       </c>
-      <c r="E6" s="29" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A7" s="29" t="s">
-        <v>344</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>343</v>
-      </c>
-      <c r="C7" s="29" t="s">
+      <c r="F7" s="29" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A8" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="D8" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="H8" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>346</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.6">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A9" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="D9" s="29" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A10" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>348</v>
-      </c>
-      <c r="C10" s="29" t="s">
+      <c r="D10" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="H10" s="29" t="s">
         <v>349</v>
       </c>
     </row>

</xml_diff>